<commit_message>
Update comments in PRODUCT_SUM xlsx test
</commit_message>
<xml_diff>
--- a/xlsx/tests/calc_tests/PRODUCT_SUM.xlsx
+++ b/xlsx/tests/calc_tests/PRODUCT_SUM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\gian\repo\IronCalc\xlsx\tests\calc_tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F1B15C1-8002-4D3B-A75F-FAC272425205}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B21D030D-9E0C-4CC8-B767-E5DB3A65BD65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" xr2:uid="{93A610EC-0ABF-4713-A1C1-0033BE11FB19}"/>
   </bookViews>
@@ -173,7 +173,7 @@
     <t>&lt;= Commented out: NotImplemented("array formulas")</t>
   </si>
   <si>
-    <t>&lt;= Returns 0 in IronCalc</t>
+    <t>&lt;= Fixed in PR #236</t>
   </si>
 </sst>
 </file>
@@ -565,7 +565,7 @@
   <dimension ref="A1:R57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -716,7 +716,7 @@
         <v>1</v>
       </c>
       <c r="B26">
-        <f>PRODUCT(A1)</f>
+        <f t="shared" ref="B26:B33" si="0">PRODUCT(A1)</f>
         <v>7</v>
       </c>
       <c r="C26">
@@ -729,7 +729,7 @@
         <v>7</v>
       </c>
       <c r="B27">
-        <f>PRODUCT(A2)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C27">
@@ -742,7 +742,7 @@
         <v>8</v>
       </c>
       <c r="B28">
-        <f>PRODUCT(A3)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C28">
@@ -755,11 +755,11 @@
         <v>22</v>
       </c>
       <c r="B29">
-        <f>PRODUCT(A4)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C29">
-        <f t="shared" ref="C29:C32" si="0">SUM(A4)</f>
+        <f t="shared" ref="C29:C32" si="1">SUM(A4)</f>
         <v>0</v>
       </c>
     </row>
@@ -768,11 +768,11 @@
         <v>23</v>
       </c>
       <c r="B30" t="e">
-        <f>PRODUCT(A5)</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="C30" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -781,11 +781,11 @@
         <v>24</v>
       </c>
       <c r="B31">
-        <f>PRODUCT(A6)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="C31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
     </row>
@@ -794,11 +794,11 @@
         <v>25</v>
       </c>
       <c r="B32">
-        <f>PRODUCT(A7)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -807,11 +807,11 @@
         <v>26</v>
       </c>
       <c r="B33">
-        <f>PRODUCT(A8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C33">
-        <f t="shared" ref="C33" si="1">SUM(A8)</f>
+        <f t="shared" ref="C33" si="2">SUM(A8)</f>
         <v>0</v>
       </c>
     </row>
@@ -833,11 +833,11 @@
         <v>13</v>
       </c>
       <c r="B35">
-        <f t="shared" ref="B35:B36" si="2">PRODUCT(A2:B2)</f>
+        <f t="shared" ref="B35:B36" si="3">PRODUCT(A2:B2)</f>
         <v>0</v>
       </c>
       <c r="C35">
-        <f t="shared" ref="C35:C36" si="3">SUM(A2:B2)</f>
+        <f t="shared" ref="C35:C36" si="4">SUM(A2:B2)</f>
         <v>0</v>
       </c>
     </row>
@@ -846,11 +846,11 @@
         <v>14</v>
       </c>
       <c r="B36">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="C36">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -859,11 +859,11 @@
         <v>28</v>
       </c>
       <c r="B37">
-        <f t="shared" ref="B37:B41" si="4">PRODUCT(A4:B4)</f>
+        <f t="shared" ref="B37:B41" si="5">PRODUCT(A4:B4)</f>
         <v>0</v>
       </c>
       <c r="C37">
-        <f t="shared" ref="C37:C41" si="5">SUM(A4:B4)</f>
+        <f t="shared" ref="C37:C41" si="6">SUM(A4:B4)</f>
         <v>0</v>
       </c>
     </row>
@@ -872,11 +872,11 @@
         <v>29</v>
       </c>
       <c r="B38" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="C38" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -885,11 +885,11 @@
         <v>30</v>
       </c>
       <c r="B39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="C39">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
     </row>
@@ -898,11 +898,11 @@
         <v>31</v>
       </c>
       <c r="B40">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="C40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -911,11 +911,11 @@
         <v>32</v>
       </c>
       <c r="B41">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="C41">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>